<commit_message>
unimpaired baseflow part 2
</commit_message>
<xml_diff>
--- a/modflow_calibration/ss_calibration/slave_dir/gage_steady_state_obs_local_flow_calc.xlsx
+++ b/modflow_calibration/ss_calibration/slave_dir/gage_steady_state_obs_local_flow_calc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\Russian_River\monte_carlo\slave_dir\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\projects\RussianRiver\RR_GSFLOW_MODEL\RR_GSFLOW\modflow_calibration\ss_calibration\slave_dir\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A005914E-E77D-42D2-A420-42817B19AD66}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2AFECF-0C0A-46C7-A179-232581A8D697}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LocalBaseflow" sheetId="4" r:id="rId1"/>

</xml_diff>